<commit_message>
Overline handling - remove char after overline, because its empty
</commit_message>
<xml_diff>
--- a/all2Unicode_v2.xlsx
+++ b/all2Unicode_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamitry/Development/coptic-font-unicode-converter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2729BDE-5A01-5442-AE3F-AD5DC3905C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA08DCC8-0685-274C-84F6-8AE2531ABAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="366" xr2:uid="{647D3334-B837-402E-9AD8-21EF25FBD15F}"/>
   </bookViews>
@@ -2995,11 +2995,11 @@
   <dimension ref="A1:AG173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="263" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F57" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I75" sqref="I75"/>
       <selection pane="topRight" activeCell="I75" sqref="I75"/>
       <selection pane="bottomLeft" activeCell="I75" sqref="I75"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="15"/>
@@ -9365,7 +9365,9 @@
       <c r="A66" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B66" s="118"/>
+      <c r="B66" s="118">
+        <v>768</v>
+      </c>
       <c r="C66" s="118" t="s">
         <v>261</v>
       </c>
@@ -9434,7 +9436,9 @@
       <c r="A67" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B67" s="118"/>
+      <c r="B67" s="118">
+        <v>773</v>
+      </c>
       <c r="C67" s="118" t="s">
         <v>262</v>
       </c>

</xml_diff>